<commit_message>
End of internship rush to finish.
</commit_message>
<xml_diff>
--- a/fft/1000Hz_charts.xlsx
+++ b/fft/1000Hz_charts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nirvanabear/Documents/code/CodeDay_Labs/Programs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nirvanabear/Documents/code/CodeDay_Labs/self-driving/fft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{7E7782B5-2FE5-2A46-A756-46322CEB5E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4027B7E9-6FA8-A94B-9FDF-A77475116CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1040" windowWidth="28800" windowHeight="16260" xr2:uid="{B55199AF-67B1-3149-9FC5-CB410D55E1E6}"/>
   </bookViews>
@@ -16,8 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$785:$J$1039</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$J$785:$J$1039</definedName>
     <definedName name="FFT_1000Hz" localSheetId="0">Sheet1!$J$2:$J$1040</definedName>
     <definedName name="FFT_serial_output" localSheetId="0">Sheet1!$B$2:$B$1298</definedName>
   </definedNames>
@@ -33,14 +31,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{7FC53DA0-E64E-8F43-B1C7-8D95AE056121}" name="FFT 1000Hz" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/nirvanabear/Documents/code/CodeDay_Labs/Programs/FFT 1000Hz.rtf" tab="0">
+    <textPr sourceFile="/Users/nirvanabear/Documents/code/CodeDay_Labs/Programs/FFT 1000Hz.rtf" tab="0">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{B9C7CEED-B240-5148-8C85-9F6C4ABA648A}" name="FFT serial output" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/nirvanabear/Documents/code/CodeDay_Labs/Programs/FFT serial output.rtf" tab="0">
+    <textPr sourceFile="/Users/nirvanabear/Documents/code/CodeDay_Labs/Programs/FFT serial output.rtf" tab="0">
       <textFields>
         <textField/>
       </textFields>
@@ -3248,8 +3246,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.4870297462817166E-2"/>
-          <c:y val="9.2986293379994173E-2"/>
+          <c:x val="1.9273462193598673E-2"/>
+          <c:y val="0.11201383463017386"/>
           <c:w val="0.89020844269466315"/>
           <c:h val="0.70844925634295708"/>
         </c:manualLayout>
@@ -8011,16 +8009,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>347133</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>67733</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2726266</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>118532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3962400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>169333</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>499533</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8083,16 +8081,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4313767</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>173567</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>143933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>766233</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>71967</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6612467</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8120,15 +8118,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>575734</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>59267</xdr:rowOff>
+      <xdr:colOff>7027334</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2675465</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>143933</xdr:rowOff>
+      <xdr:colOff>2159000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>8468</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8155,16 +8153,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>753534</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>156632</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>448734</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>21165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>6015567</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>927101</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8499,8 +8497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8149B-2B3C-1944-8EF6-23BB7CED26B6}">
   <dimension ref="B2:J1298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>